<commit_message>
update blank out of test data
update blank out of test data
</commit_message>
<xml_diff>
--- a/test/_unittest/testdata/testdata.xlsx
+++ b/test/_unittest/testdata/testdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2070812\OneDrive - Cognizant\Documents\GitHub\playwright-bdd\test\_unittest\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E4088C-86A6-46A6-A1F5-0DE69E997DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15660" tabRatio="664" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="664" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="70">
   <si>
     <t>Id</t>
   </si>
@@ -237,23 +243,20 @@
     <t>Infostretch Test Automation Framework3</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
+    <t xml:space="preserve">  start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -268,159 +271,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,192 +281,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -622,313 +294,28 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1186,22 +573,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0735294117647" defaultRowHeight="17.6" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="8.46323529411765" customWidth="1"/>
-    <col min="7" max="7" width="17.1544117647059" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1244,7 +631,7 @@
         <v>44256</v>
       </c>
       <c r="F2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G2" t="str">
         <f>LOWER(CONCATENATE(B2,".",C2,"@test.com"))</f>
@@ -1326,23 +713,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0735294117647" defaultRowHeight="17.6" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="8.46323529411765" customWidth="1"/>
-    <col min="7" max="7" width="17.1544117647059" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1385,7 +768,7 @@
         <v>44256</v>
       </c>
       <c r="F2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G2" t="str">
         <f>LOWER(CONCATENATE(B2,".",C2,"@test.com"))</f>
@@ -1467,29 +850,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B7:T39"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0735294117647" defaultRowHeight="17.6"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="9" max="9" width="17.6911764705882" customWidth="1"/>
-    <col min="10" max="10" width="19.1544117647059" customWidth="1"/>
-    <col min="15" max="15" width="13.8455882352941" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" customWidth="1"/>
     <col min="16" max="16" width="24" customWidth="1"/>
     <col min="19" max="19" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:10">
+    <row r="7" spans="3:11">
       <c r="C7" t="s">
         <v>15</v>
       </c>
@@ -1515,7 +896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="4:10">
+    <row r="8" spans="3:11">
       <c r="D8" s="2">
         <v>1</v>
       </c>
@@ -1532,14 +913,14 @@
         <v>44256</v>
       </c>
       <c r="I8" s="2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J8" s="2" t="str">
         <f>LOWER(CONCATENATE(E8,".",F8,"@test.com"))</f>
         <v>test1.l1@test.com</v>
       </c>
     </row>
-    <row r="9" spans="4:10">
+    <row r="9" spans="3:11">
       <c r="D9" s="2">
         <v>2</v>
       </c>
@@ -1563,7 +944,7 @@
         <v>test2.l2@test.com</v>
       </c>
     </row>
-    <row r="10" spans="4:10">
+    <row r="10" spans="3:11">
       <c r="D10" s="2">
         <v>3</v>
       </c>
@@ -1587,7 +968,7 @@
         <v>test3.l3@test.com</v>
       </c>
     </row>
-    <row r="11" spans="4:11">
+    <row r="11" spans="3:11">
       <c r="D11" s="2">
         <v>4</v>
       </c>
@@ -1614,7 +995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="9:17">
+    <row r="19" spans="3:17">
       <c r="I19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1641,7 +1022,7 @@
       </c>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="9:17">
+    <row r="20" spans="3:17">
       <c r="I20" s="2"/>
       <c r="J20" s="2">
         <v>5</v>
@@ -1667,7 +1048,7 @@
       </c>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="9:17">
+    <row r="21" spans="3:17">
       <c r="I21" s="2"/>
       <c r="J21" s="2">
         <v>6</v>
@@ -1693,7 +1074,7 @@
       </c>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="9:17">
+    <row r="22" spans="3:17">
       <c r="I22" s="2"/>
       <c r="J22" s="2">
         <v>7</v>
@@ -1719,7 +1100,7 @@
       </c>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="9:17">
+    <row r="23" spans="3:17">
       <c r="I23" s="2"/>
       <c r="J23" s="2">
         <v>8</v>
@@ -1747,7 +1128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="3:11">
+    <row r="27" spans="3:17">
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1774,7 +1155,7 @@
       </c>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="3:11">
+    <row r="28" spans="3:17">
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <v>9</v>
@@ -1800,7 +1181,7 @@
       </c>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="3:11">
+    <row r="29" spans="3:17">
       <c r="C29" s="2"/>
       <c r="D29" s="2">
         <v>10</v>
@@ -1826,7 +1207,7 @@
       </c>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="3:11">
+    <row r="30" spans="3:17">
       <c r="C30" s="2"/>
       <c r="D30" s="2">
         <v>11</v>
@@ -1852,7 +1233,7 @@
       </c>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="3:11">
+    <row r="31" spans="3:17">
       <c r="C31" s="2"/>
       <c r="D31" s="2">
         <v>12</v>
@@ -1870,7 +1251,7 @@
         <v>44267</v>
       </c>
       <c r="I31" s="2">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J31" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1950,7 +1331,7 @@
         <v>44268</v>
       </c>
       <c r="H36" s="2">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I36" s="2" t="str">
         <f>LOWER(CONCATENATE(D36,".",E36,"@test.com"))</f>
@@ -2139,26 +1520,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7647058823529" customWidth="1"/>
-    <col min="2" max="2" width="34.1544117647059" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -2169,7 +1548,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -2197,30 +1576,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" width="13.7647058823529" customWidth="1"/>
-    <col min="3" max="3" width="34.1544117647059" customWidth="1"/>
-    <col min="4" max="4" width="7.38235294117647" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.4140625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="34.1544117647059" customWidth="1"/>
-    <col min="10" max="10" width="7.38235294117647" customWidth="1"/>
+    <col min="9" max="9" width="34.1640625" customWidth="1"/>
+    <col min="10" max="10" width="7.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -2234,7 +1611,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="1:11">
       <c r="B3" s="2" t="s">
         <v>55</v>
       </c>
@@ -2245,7 +1622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="1:11">
       <c r="B4" s="2" t="s">
         <v>57</v>
       </c>
@@ -2259,7 +1636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="7:10">
+    <row r="11" spans="1:11">
       <c r="G11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2273,7 +1650,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="8:10">
+    <row r="12" spans="1:11">
       <c r="H12" s="2" t="s">
         <v>59</v>
       </c>
@@ -2284,7 +1661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="8:11">
+    <row r="13" spans="1:11">
       <c r="H13" s="2" t="s">
         <v>61</v>
       </c>
@@ -2298,7 +1675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="7:10">
+    <row r="23" spans="7:11">
       <c r="G23" s="2" t="s">
         <v>25</v>
       </c>
@@ -2312,7 +1689,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="8:10">
+    <row r="24" spans="7:11">
       <c r="H24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2323,7 +1700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="8:11">
+    <row r="25" spans="7:11">
       <c r="H25" s="2" t="s">
         <v>65</v>
       </c>
@@ -2339,23 +1716,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6" outlineLevelRow="2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7647058823529" customWidth="1"/>
-    <col min="2" max="2" width="34.1544117647059" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2393,22 +1768,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2416,7 +1789,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2424,7 +1797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2432,7 +1805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2440,25 +1813,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="C5" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0735294117647" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="11.08203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="8.46323529411765" customWidth="1"/>
-    <col min="7" max="7" width="17.1544117647059" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2502,7 +1878,7 @@
         <v>45042</v>
       </c>
       <c r="F2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G4" si="0">LOWER(CONCATENATE(B2,".",C2,"@test.com"))</f>
@@ -2560,6 +1936,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>